<commit_message>
jalon 3 fait + jalon 2 mise a jour
</commit_message>
<xml_diff>
--- a/outputs/results/results_instance_WPY_realiste_jalon2_voies.xlsx
+++ b/outputs/results/results_instance_WPY_realiste_jalon2_voies.xlsx
@@ -457,10 +457,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>66.66666666666667</v>
+        <v>86.66666666666667</v>
       </c>
       <c r="C2" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D2" t="n">
         <v>15</v>
@@ -473,10 +473,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>7.5</v>
+        <v>20</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D3" t="n">
         <v>40</v>
@@ -489,10 +489,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>92.85714285714286</v>
+        <v>100</v>
       </c>
       <c r="C4" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" t="n">
         <v>14</v>

</xml_diff>